<commit_message>
can now choose to save pca/tsne
</commit_message>
<xml_diff>
--- a/results/Results.xlsx
+++ b/results/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>0.1607</t>
+  </si>
+  <si>
+    <t>0.8027</t>
+  </si>
+  <si>
+    <t>0.2953</t>
+  </si>
+  <si>
+    <t>0.0990</t>
   </si>
 </sst>
 </file>
@@ -255,6 +264,48 @@
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -268,48 +319,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -592,181 +601,190 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="13"/>
-    <col min="2" max="4" width="10.83203125" style="14"/>
-    <col min="5" max="5" width="15.6640625" style="15" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" style="15" customWidth="1"/>
-    <col min="7" max="8" width="10.83203125" style="15"/>
-    <col min="9" max="9" width="10.83203125" style="16"/>
-    <col min="10" max="10" width="10.83203125" style="17"/>
-    <col min="11" max="11" width="13.6640625" style="17" customWidth="1"/>
-    <col min="12" max="12" width="10.83203125" style="17"/>
-    <col min="13" max="13" width="31.6640625" style="17" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" style="19" customWidth="1"/>
-    <col min="15" max="15" width="15.1640625" style="19" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="8"/>
+    <col min="2" max="4" width="10.83203125" style="9"/>
+    <col min="5" max="5" width="15.6640625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" style="10" customWidth="1"/>
+    <col min="7" max="8" width="10.83203125" style="10"/>
+    <col min="9" max="9" width="10.83203125" style="11"/>
+    <col min="10" max="10" width="10.83203125" style="12"/>
+    <col min="11" max="11" width="13.6640625" style="12" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" style="12"/>
+    <col min="13" max="13" width="31.6640625" style="12" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" style="14" customWidth="1"/>
+    <col min="15" max="15" width="15.1640625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="3" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="5" t="s">
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="5"/>
+      <c r="O1" s="19"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="13">
+      <c r="A3" s="8">
         <v>1645</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="10">
         <v>10</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="10">
         <v>100</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="10">
         <v>0</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="10">
         <v>750</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="17">
+      <c r="J3" s="12">
         <v>1</v>
       </c>
-      <c r="K3" s="18">
+      <c r="K3" s="13">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="L3" s="17">
+      <c r="L3" s="12">
         <v>50</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="19">
+      <c r="N3" s="14">
         <v>10000</v>
       </c>
-      <c r="O3" s="19" t="s">
+      <c r="O3" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="13">
+      <c r="A4" s="8">
         <v>2235</v>
       </c>
-      <c r="E4" s="15">
+      <c r="B4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="15">
+      <c r="E4" s="10">
+        <v>30</v>
+      </c>
+      <c r="F4" s="10">
         <v>100</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="10">
         <v>0</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="10">
         <v>750</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J4" s="12">
         <v>1</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="13">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="L4" s="17">
+      <c r="L4" s="12">
         <v>50</v>
       </c>
-      <c r="M4" s="17" t="s">
+      <c r="M4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="19">
+      <c r="N4" s="14">
         <v>10000</v>
       </c>
-      <c r="O4" s="19" t="s">
+      <c r="O4" s="14" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated gitignore to add ~.xlsl
</commit_message>
<xml_diff>
--- a/results/Results.xlsx
+++ b/results/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>0.0990</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>90-10-0</t>
   </si>
 </sst>
 </file>
@@ -598,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -788,6 +794,26 @@
         <v>23</v>
       </c>
     </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="10">
+        <v>10</v>
+      </c>
+      <c r="F5" s="10">
+        <v>100</v>
+      </c>
+      <c r="G5" s="10">
+        <v>0</v>
+      </c>
+      <c r="H5" s="10">
+        <v>1500</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B1:D1"/>

</xml_diff>